<commit_message>
Update LHV of fuels
</commit_message>
<xml_diff>
--- a/dev/Input data.xlsx
+++ b/dev/Input data.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Vehicle parameters'!$A$2:$AB$209</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcMode="manual" iterate="1" iterateCount="15" iterateDelta="0.01"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -410,18 +410,10 @@
 And a 400kW motor from Wolff et al. 2020</t>
   </si>
   <si>
-    <t>https://batteryuniversity.com/learn/article/fuel_cell_technology</t>
-  </si>
-  <si>
     <t>hours</t>
   </si>
   <si>
     <t>fuel cell lifetime hours</t>
-  </si>
-  <si>
-    <t>Between 2000 and 4000 hours for passenger cars.
-For MDV and HDV, FC are assumed to be sturdier and used at lower intenisty.
-Hence, around 5000 hours in 2020, 7000 hours in 2050.</t>
   </si>
   <si>
     <t>number of axles</t>
@@ -900,6 +892,12 @@
   </si>
   <si>
     <t>battery cell energy density, NMC</t>
+  </si>
+  <si>
+    <t>https://www.nrel.gov/docs/fy21osti/75583.pdf</t>
+  </si>
+  <si>
+    <t>Around 17,000 hours on average to reach 20% cell voltage degradation. DoE's ultimate target is 25,000 hours, which we set for 2050.</t>
   </si>
 </sst>
 </file>
@@ -1440,7 +1438,7 @@
       <pane xSplit="10" ySplit="2" topLeftCell="K40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D69" sqref="D69"/>
+      <selection pane="bottomRight" activeCell="H210" sqref="H210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1613,10 +1611,10 @@
         <v>20</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>82</v>
@@ -1628,7 +1626,7 @@
         <v>58</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>50</v>
@@ -1697,10 +1695,10 @@
         <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>82</v>
@@ -1712,10 +1710,10 @@
         <v>58</v>
       </c>
       <c r="H4" s="27" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>50</v>
@@ -1783,10 +1781,10 @@
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>82</v>
@@ -1798,10 +1796,10 @@
         <v>58</v>
       </c>
       <c r="H5" s="27" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>50</v>
@@ -1869,10 +1867,10 @@
         <v>20</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>82</v>
@@ -1884,10 +1882,10 @@
         <v>58</v>
       </c>
       <c r="H6" s="27" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>50</v>
@@ -1958,10 +1956,10 @@
         <v>20</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>61</v>
@@ -1970,10 +1968,10 @@
         <v>58</v>
       </c>
       <c r="H7" s="27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>88</v>
@@ -2020,10 +2018,10 @@
         <v>20</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>61</v>
@@ -2032,10 +2030,10 @@
         <v>58</v>
       </c>
       <c r="H8" s="27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>88</v>
@@ -2076,13 +2074,13 @@
         <v>23</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>74</v>
@@ -2093,7 +2091,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="27"/>
       <c r="I9" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>88</v>
@@ -2134,13 +2132,13 @@
         <v>23</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>74</v>
@@ -2151,7 +2149,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="27"/>
       <c r="I10" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>88</v>
@@ -2192,13 +2190,13 @@
         <v>23</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>74</v>
@@ -2209,7 +2207,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="27"/>
       <c r="I11" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>88</v>
@@ -2253,10 +2251,10 @@
         <v>20</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>74</v>
@@ -2267,7 +2265,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="27"/>
       <c r="I12" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>88</v>
@@ -2311,10 +2309,10 @@
         <v>20</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>74</v>
@@ -2325,7 +2323,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="27"/>
       <c r="I13" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>88</v>
@@ -2366,13 +2364,13 @@
         <v>23</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>74</v>
@@ -2384,10 +2382,10 @@
         <v>58</v>
       </c>
       <c r="H14" s="27" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>50</v>
@@ -2452,13 +2450,13 @@
         <v>23</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>74</v>
@@ -2470,10 +2468,10 @@
         <v>58</v>
       </c>
       <c r="H15" s="27" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>50</v>
@@ -2538,13 +2536,13 @@
         <v>23</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>74</v>
@@ -2557,7 +2555,7 @@
       </c>
       <c r="H16" s="27"/>
       <c r="I16" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>50</v>
@@ -2622,13 +2620,13 @@
         <v>23</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>74</v>
@@ -2641,7 +2639,7 @@
       </c>
       <c r="H17" s="27"/>
       <c r="I17" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>50</v>
@@ -2709,10 +2707,10 @@
         <v>20</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>82</v>
@@ -2724,10 +2722,10 @@
         <v>58</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>50</v>
@@ -2807,10 +2805,10 @@
         <v>20</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>82</v>
@@ -2822,10 +2820,10 @@
         <v>58</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>50</v>
@@ -2905,10 +2903,10 @@
         <v>20</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>82</v>
@@ -2920,10 +2918,10 @@
         <v>58</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>50</v>
@@ -3000,13 +2998,13 @@
         <v>23</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>82</v>
@@ -3018,10 +3016,10 @@
         <v>58</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>50</v>
@@ -3098,13 +3096,13 @@
         <v>23</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>82</v>
@@ -3116,10 +3114,10 @@
         <v>58</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>50</v>
@@ -3199,7 +3197,7 @@
         <v>20</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>2</v>
@@ -3214,10 +3212,10 @@
         <v>58</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>50</v>
@@ -3297,7 +3295,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>2</v>
@@ -3312,10 +3310,10 @@
         <v>58</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>50</v>
@@ -3395,7 +3393,7 @@
         <v>20</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>2</v>
@@ -3410,10 +3408,10 @@
         <v>58</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>50</v>
@@ -3493,7 +3491,7 @@
         <v>20</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>46</v>
@@ -3508,10 +3506,10 @@
         <v>58</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>50</v>
@@ -3591,7 +3589,7 @@
         <v>20</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>46</v>
@@ -3606,10 +3604,10 @@
         <v>58</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>50</v>
@@ -3689,7 +3687,7 @@
         <v>20</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>46</v>
@@ -3704,10 +3702,10 @@
         <v>58</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>50</v>
@@ -3784,16 +3782,16 @@
         <v>29</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>60</v>
@@ -3803,7 +3801,7 @@
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>88</v>
@@ -3844,16 +3842,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>60</v>
@@ -3863,7 +3861,7 @@
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>88</v>
@@ -3907,13 +3905,13 @@
         <v>20</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>60</v>
@@ -3923,7 +3921,7 @@
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>88</v>
@@ -3964,13 +3962,13 @@
         <v>29</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C32" s="28" t="s">
         <v>20</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>77</v>
@@ -3983,7 +3981,7 @@
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J32" s="3" t="s">
         <v>88</v>
@@ -4278,7 +4276,7 @@
         <v>31</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>20</v>
@@ -4360,7 +4358,7 @@
         <v>24</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>20</v>
@@ -4620,7 +4618,7 @@
         <v>24</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>20</v>
@@ -4708,10 +4706,10 @@
         <v>20</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>60</v>
@@ -4720,67 +4718,67 @@
         <v>58</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>124</v>
+        <v>284</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>127</v>
+        <v>285</v>
       </c>
       <c r="J42" s="3" t="s">
         <v>50</v>
       </c>
       <c r="K42" s="5">
-        <v>4000</v>
+        <v>80000</v>
       </c>
       <c r="L42" s="5">
-        <v>3500</v>
+        <v>5000</v>
       </c>
       <c r="M42" s="5">
-        <v>4500</v>
+        <v>10000</v>
       </c>
       <c r="N42" s="5">
-        <v>4500</v>
+        <v>12000</v>
       </c>
       <c r="O42" s="5">
-        <v>4000</v>
+        <v>10000</v>
       </c>
       <c r="P42" s="5">
-        <v>5000</v>
+        <v>15000</v>
       </c>
       <c r="Q42" s="1">
-        <v>5000</v>
+        <v>17000</v>
       </c>
       <c r="R42" s="5">
-        <v>4500</v>
+        <v>15000</v>
       </c>
       <c r="S42" s="5">
-        <v>5500</v>
+        <v>20000</v>
       </c>
       <c r="T42" s="5">
-        <v>5500</v>
+        <v>20000</v>
       </c>
       <c r="U42" s="5">
-        <v>5000</v>
+        <v>17000</v>
       </c>
       <c r="V42" s="5">
-        <v>6000</v>
+        <v>23000</v>
       </c>
       <c r="W42" s="5">
-        <v>6000</v>
+        <v>22500</v>
       </c>
       <c r="X42" s="5">
-        <v>5500</v>
+        <v>20000</v>
       </c>
       <c r="Y42" s="5">
-        <v>6500</v>
+        <v>25000</v>
       </c>
       <c r="Z42" s="3">
-        <v>6500</v>
+        <v>25000</v>
       </c>
       <c r="AA42" s="3">
-        <v>6000</v>
+        <v>22500</v>
       </c>
       <c r="AB42" s="3">
-        <v>7000</v>
+        <v>27500</v>
       </c>
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.3">
@@ -5048,7 +5046,7 @@
         <v>20</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>77</v>
@@ -5058,10 +5056,10 @@
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J46" s="3" t="s">
         <v>50</v>
@@ -5081,7 +5079,7 @@
         <v>2000</v>
       </c>
       <c r="O46" s="5">
-        <f t="shared" ref="O46:AB46" si="28">N46*0.75</f>
+        <f t="shared" ref="O46" si="28">N46*0.75</f>
         <v>1500</v>
       </c>
       <c r="P46" s="5">
@@ -5092,7 +5090,7 @@
         <v>2000</v>
       </c>
       <c r="R46" s="5">
-        <f t="shared" ref="R46:AB46" si="30">Q46*0.75</f>
+        <f t="shared" ref="R46" si="30">Q46*0.75</f>
         <v>1500</v>
       </c>
       <c r="S46" s="5">
@@ -5103,7 +5101,7 @@
         <v>2000</v>
       </c>
       <c r="U46" s="5">
-        <f t="shared" ref="U46:AB46" si="32">T46*0.75</f>
+        <f t="shared" ref="U46" si="32">T46*0.75</f>
         <v>1500</v>
       </c>
       <c r="V46" s="5">
@@ -5114,7 +5112,7 @@
         <v>2000</v>
       </c>
       <c r="X46" s="5">
-        <f t="shared" ref="X46:AB46" si="34">W46*0.75</f>
+        <f t="shared" ref="X46" si="34">W46*0.75</f>
         <v>1500</v>
       </c>
       <c r="Y46" s="5">
@@ -5125,7 +5123,7 @@
         <v>2000</v>
       </c>
       <c r="AA46" s="5">
-        <f t="shared" ref="AA46:AB46" si="36">Z46*0.75</f>
+        <f t="shared" ref="AA46" si="36">Z46*0.75</f>
         <v>1500</v>
       </c>
       <c r="AB46" s="5">
@@ -5144,7 +5142,7 @@
         <v>20</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>77</v>
@@ -5154,10 +5152,10 @@
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J47" s="3" t="s">
         <v>50</v>
@@ -5177,7 +5175,7 @@
         <v>1000</v>
       </c>
       <c r="O47" s="5">
-        <f t="shared" ref="O47:AB47" si="38">N47*0.75</f>
+        <f t="shared" ref="O47" si="38">N47*0.75</f>
         <v>750</v>
       </c>
       <c r="P47" s="5">
@@ -5188,7 +5186,7 @@
         <v>1000</v>
       </c>
       <c r="R47" s="5">
-        <f t="shared" ref="R47:AB47" si="39">Q47*0.75</f>
+        <f t="shared" ref="R47" si="39">Q47*0.75</f>
         <v>750</v>
       </c>
       <c r="S47" s="5">
@@ -5199,7 +5197,7 @@
         <v>1000</v>
       </c>
       <c r="U47" s="5">
-        <f t="shared" ref="U47:AB47" si="40">T47*0.75</f>
+        <f t="shared" ref="U47" si="40">T47*0.75</f>
         <v>750</v>
       </c>
       <c r="V47" s="5">
@@ -5210,7 +5208,7 @@
         <v>1000</v>
       </c>
       <c r="X47" s="5">
-        <f t="shared" ref="X47:AB47" si="41">W47*0.75</f>
+        <f t="shared" ref="X47" si="41">W47*0.75</f>
         <v>750</v>
       </c>
       <c r="Y47" s="5">
@@ -5221,7 +5219,7 @@
         <v>1000</v>
       </c>
       <c r="AA47" s="5">
-        <f t="shared" ref="AA47:AB47" si="42">Z47*0.75</f>
+        <f t="shared" ref="AA47" si="42">Z47*0.75</f>
         <v>750</v>
       </c>
       <c r="AB47" s="5">
@@ -5240,7 +5238,7 @@
         <v>20</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E48" s="8" t="s">
         <v>77</v>
@@ -5250,10 +5248,10 @@
       </c>
       <c r="G48" s="3"/>
       <c r="H48" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J48" s="3" t="s">
         <v>50</v>
@@ -5273,7 +5271,7 @@
         <v>7000</v>
       </c>
       <c r="O48" s="5">
-        <f t="shared" ref="O48:AB48" si="43">N48*0.75</f>
+        <f t="shared" ref="O48" si="43">N48*0.75</f>
         <v>5250</v>
       </c>
       <c r="P48" s="5">
@@ -5284,7 +5282,7 @@
         <v>7000</v>
       </c>
       <c r="R48" s="5">
-        <f t="shared" ref="R48:AB48" si="44">Q48*0.75</f>
+        <f t="shared" ref="R48" si="44">Q48*0.75</f>
         <v>5250</v>
       </c>
       <c r="S48" s="5">
@@ -5295,7 +5293,7 @@
         <v>7000</v>
       </c>
       <c r="U48" s="5">
-        <f t="shared" ref="U48:AB48" si="45">T48*0.75</f>
+        <f t="shared" ref="U48" si="45">T48*0.75</f>
         <v>5250</v>
       </c>
       <c r="V48" s="5">
@@ -5306,7 +5304,7 @@
         <v>7000</v>
       </c>
       <c r="X48" s="5">
-        <f t="shared" ref="X48:AB48" si="46">W48*0.75</f>
+        <f t="shared" ref="X48" si="46">W48*0.75</f>
         <v>5250</v>
       </c>
       <c r="Y48" s="5">
@@ -5317,7 +5315,7 @@
         <v>7000</v>
       </c>
       <c r="AA48" s="5">
-        <f t="shared" ref="AA48:AB48" si="47">Z48*0.75</f>
+        <f t="shared" ref="AA48" si="47">Z48*0.75</f>
         <v>5250</v>
       </c>
       <c r="AB48" s="5">
@@ -5336,7 +5334,7 @@
         <v>20</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>77</v>
@@ -5346,10 +5344,10 @@
       </c>
       <c r="G49" s="3"/>
       <c r="H49" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J49" s="3" t="s">
         <v>50</v>
@@ -5369,7 +5367,7 @@
         <v>7000</v>
       </c>
       <c r="O49" s="5">
-        <f t="shared" ref="O49:AB49" si="48">N49*0.75</f>
+        <f t="shared" ref="O49" si="48">N49*0.75</f>
         <v>5250</v>
       </c>
       <c r="P49" s="5">
@@ -5380,7 +5378,7 @@
         <v>7000</v>
       </c>
       <c r="R49" s="5">
-        <f t="shared" ref="R49:AB49" si="49">Q49*0.75</f>
+        <f t="shared" ref="R49" si="49">Q49*0.75</f>
         <v>5250</v>
       </c>
       <c r="S49" s="5">
@@ -5391,7 +5389,7 @@
         <v>7000</v>
       </c>
       <c r="U49" s="5">
-        <f t="shared" ref="U49:AB49" si="50">T49*0.75</f>
+        <f t="shared" ref="U49" si="50">T49*0.75</f>
         <v>5250</v>
       </c>
       <c r="V49" s="5">
@@ -5402,7 +5400,7 @@
         <v>7000</v>
       </c>
       <c r="X49" s="5">
-        <f t="shared" ref="X49:AB49" si="51">W49*0.75</f>
+        <f t="shared" ref="X49" si="51">W49*0.75</f>
         <v>5250</v>
       </c>
       <c r="Y49" s="5">
@@ -5413,7 +5411,7 @@
         <v>7000</v>
       </c>
       <c r="AA49" s="5">
-        <f t="shared" ref="AA49:AB49" si="52">Z49*0.75</f>
+        <f t="shared" ref="AA49" si="52">Z49*0.75</f>
         <v>5250</v>
       </c>
       <c r="AB49" s="5">
@@ -5426,7 +5424,7 @@
         <v>24</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>20</v>
@@ -5512,13 +5510,13 @@
         <v>24</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E51" s="8" t="s">
         <v>74</v>
@@ -5530,10 +5528,10 @@
         <v>59</v>
       </c>
       <c r="H51" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="J51" s="3" t="s">
         <v>88</v>
@@ -5574,7 +5572,7 @@
         <v>24</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>20</v>
@@ -5592,10 +5590,10 @@
         <v>59</v>
       </c>
       <c r="H52" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="J52" s="3" t="s">
         <v>50</v>
@@ -5672,7 +5670,7 @@
         <v>24</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>20</v>
@@ -5690,10 +5688,10 @@
         <v>59</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J53" s="3" t="s">
         <v>50</v>
@@ -5782,10 +5780,10 @@
         <v>59</v>
       </c>
       <c r="H54" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="I54" s="3" t="s">
         <v>227</v>
-      </c>
-      <c r="I54" s="3" t="s">
-        <v>229</v>
       </c>
       <c r="J54" s="3" t="s">
         <v>88</v>
@@ -5826,13 +5824,13 @@
         <v>24</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>74</v>
@@ -5844,10 +5842,10 @@
         <v>58</v>
       </c>
       <c r="H55" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="I55" s="3" t="s">
         <v>236</v>
-      </c>
-      <c r="I55" s="3" t="s">
-        <v>238</v>
       </c>
       <c r="J55" s="3" t="s">
         <v>50</v>
@@ -5912,13 +5910,13 @@
         <v>24</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>74</v>
@@ -5930,10 +5928,10 @@
         <v>58</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J56" s="3" t="s">
         <v>50</v>
@@ -5998,7 +5996,7 @@
         <v>24</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>20</v>
@@ -6016,10 +6014,10 @@
         <v>59</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J57" s="3" t="s">
         <v>50</v>
@@ -6090,7 +6088,7 @@
         <v>24</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>20</v>
@@ -6111,7 +6109,7 @@
         <v>55</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J58" s="3" t="s">
         <v>50</v>
@@ -6182,7 +6180,7 @@
         <v>24</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>20</v>
@@ -6274,7 +6272,7 @@
         <v>24</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>20</v>
@@ -6446,7 +6444,7 @@
         <v>24</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>20</v>
@@ -6618,7 +6616,7 @@
         <v>24</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>20</v>
@@ -6710,7 +6708,7 @@
         <v>24</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>20</v>
@@ -6974,7 +6972,7 @@
         <v>20</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>83</v>
@@ -7058,7 +7056,7 @@
         <v>20</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E69" s="8" t="s">
         <v>83</v>
@@ -7142,7 +7140,7 @@
         <v>20</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E70" s="8" t="s">
         <v>83</v>
@@ -7238,7 +7236,7 @@
         <v>20</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>83</v>
@@ -7250,7 +7248,7 @@
         <v>59</v>
       </c>
       <c r="H71" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I71" s="3"/>
       <c r="J71" s="3" t="s">
@@ -7328,13 +7326,13 @@
         <v>24</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E72" s="8" t="s">
         <v>82</v>
@@ -7346,10 +7344,10 @@
         <v>59</v>
       </c>
       <c r="H72" s="7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I72" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="J72" s="3" t="s">
         <v>88</v>
@@ -7390,13 +7388,13 @@
         <v>24</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E73" s="8" t="s">
         <v>82</v>
@@ -7409,7 +7407,7 @@
       </c>
       <c r="H73" s="7"/>
       <c r="I73" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J73" s="3" t="s">
         <v>88</v>
@@ -7450,13 +7448,13 @@
         <v>24</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E74" s="8" t="s">
         <v>74</v>
@@ -7468,10 +7466,10 @@
         <v>59</v>
       </c>
       <c r="H74" s="7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="J74" s="3" t="s">
         <v>50</v>
@@ -7541,10 +7539,10 @@
         <v>20</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>77</v>
@@ -7556,7 +7554,7 @@
         <v>57</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J75" s="16" t="s">
         <v>88</v>
@@ -7600,10 +7598,10 @@
         <v>20</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>77</v>
@@ -7615,7 +7613,7 @@
         <v>57</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J76" s="16" t="s">
         <v>88</v>
@@ -7659,7 +7657,7 @@
         <v>20</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D77" s="19" t="s">
         <v>112</v>
@@ -7677,7 +7675,7 @@
         <v>96</v>
       </c>
       <c r="I77" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J77" s="19" t="s">
         <v>50</v>
@@ -7757,7 +7755,7 @@
         <v>20</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D78" s="19" t="s">
         <v>112</v>
@@ -7775,7 +7773,7 @@
         <v>96</v>
       </c>
       <c r="I78" s="19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J78" s="19" t="s">
         <v>50</v>
@@ -7855,7 +7853,7 @@
         <v>20</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D79" s="19" t="s">
         <v>112</v>
@@ -7873,7 +7871,7 @@
         <v>96</v>
       </c>
       <c r="I79" s="19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J79" s="19" t="s">
         <v>50</v>
@@ -7953,7 +7951,7 @@
         <v>20</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D80" s="19" t="s">
         <v>112</v>
@@ -7971,7 +7969,7 @@
         <v>96</v>
       </c>
       <c r="I80" s="19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J80" s="19" t="s">
         <v>50</v>
@@ -8051,7 +8049,7 @@
         <v>20</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D81" s="19" t="s">
         <v>112</v>
@@ -8069,7 +8067,7 @@
         <v>96</v>
       </c>
       <c r="I81" s="19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J81" s="19" t="s">
         <v>50</v>
@@ -8149,7 +8147,7 @@
         <v>20</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D82" s="19" t="s">
         <v>112</v>
@@ -8167,7 +8165,7 @@
         <v>96</v>
       </c>
       <c r="I82" s="19" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J82" s="19" t="s">
         <v>50</v>
@@ -8247,7 +8245,7 @@
         <v>20</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D83" s="19" t="s">
         <v>110</v>
@@ -8265,7 +8263,7 @@
         <v>96</v>
       </c>
       <c r="I83" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J83" s="19" t="s">
         <v>50</v>
@@ -8345,7 +8343,7 @@
         <v>20</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D84" s="19" t="s">
         <v>110</v>
@@ -8363,7 +8361,7 @@
         <v>96</v>
       </c>
       <c r="I84" s="19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J84" s="19" t="s">
         <v>50</v>
@@ -8443,7 +8441,7 @@
         <v>20</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D85" s="19" t="s">
         <v>110</v>
@@ -8461,7 +8459,7 @@
         <v>96</v>
       </c>
       <c r="I85" s="19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J85" s="19" t="s">
         <v>50</v>
@@ -8541,7 +8539,7 @@
         <v>20</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D86" s="19" t="s">
         <v>110</v>
@@ -8559,7 +8557,7 @@
         <v>96</v>
       </c>
       <c r="I86" s="19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J86" s="19" t="s">
         <v>50</v>
@@ -8639,7 +8637,7 @@
         <v>20</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D87" s="19" t="s">
         <v>110</v>
@@ -8657,7 +8655,7 @@
         <v>96</v>
       </c>
       <c r="I87" s="19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J87" s="19" t="s">
         <v>50</v>
@@ -8737,7 +8735,7 @@
         <v>20</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D88" s="19" t="s">
         <v>110</v>
@@ -8755,7 +8753,7 @@
         <v>96</v>
       </c>
       <c r="I88" s="19" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J88" s="19" t="s">
         <v>50</v>
@@ -8916,10 +8914,10 @@
         <v>21</v>
       </c>
       <c r="B90" s="19" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D90" s="8" t="s">
         <v>0</v>
@@ -9018,10 +9016,10 @@
         <v>21</v>
       </c>
       <c r="B91" s="19" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D91" s="8" t="s">
         <v>0</v>
@@ -9120,10 +9118,10 @@
         <v>21</v>
       </c>
       <c r="B92" s="19" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D92" s="8" t="s">
         <v>0</v>
@@ -9222,10 +9220,10 @@
         <v>21</v>
       </c>
       <c r="B93" s="19" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D93" s="8" t="s">
         <v>0</v>
@@ -9324,10 +9322,10 @@
         <v>21</v>
       </c>
       <c r="B94" s="19" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D94" s="8" t="s">
         <v>0</v>
@@ -9426,10 +9424,10 @@
         <v>21</v>
       </c>
       <c r="B95" s="19" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D95" s="8" t="s">
         <v>0</v>
@@ -9528,10 +9526,10 @@
         <v>21</v>
       </c>
       <c r="B96" s="19" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D96" s="8" t="s">
         <v>0</v>
@@ -9630,10 +9628,10 @@
         <v>21</v>
       </c>
       <c r="B97" s="19" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D97" s="8" t="s">
         <v>0</v>
@@ -9732,10 +9730,10 @@
         <v>21</v>
       </c>
       <c r="B98" s="19" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D98" s="8" t="s">
         <v>0</v>
@@ -9834,10 +9832,10 @@
         <v>21</v>
       </c>
       <c r="B99" s="19" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D99" s="8" t="s">
         <v>0</v>
@@ -9936,10 +9934,10 @@
         <v>21</v>
       </c>
       <c r="B100" s="19" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D100" s="8" t="s">
         <v>0</v>
@@ -10038,10 +10036,10 @@
         <v>21</v>
       </c>
       <c r="B101" s="19" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D101" s="8" t="s">
         <v>0</v>
@@ -10143,7 +10141,7 @@
         <v>20</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>104</v>
@@ -10201,7 +10199,7 @@
         <v>20</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>104</v>
@@ -10259,7 +10257,7 @@
         <v>20</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>104</v>
@@ -10317,7 +10315,7 @@
         <v>20</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>104</v>
@@ -10375,7 +10373,7 @@
         <v>20</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D106" s="19" t="s">
         <v>17</v>
@@ -10393,7 +10391,7 @@
         <v>96</v>
       </c>
       <c r="I106" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J106" s="3" t="s">
         <v>50</v>
@@ -10473,7 +10471,7 @@
         <v>20</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D107" s="19" t="s">
         <v>17</v>
@@ -10491,7 +10489,7 @@
         <v>96</v>
       </c>
       <c r="I107" s="19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J107" s="3" t="s">
         <v>50</v>
@@ -10571,7 +10569,7 @@
         <v>20</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D108" s="19" t="s">
         <v>17</v>
@@ -10589,7 +10587,7 @@
         <v>96</v>
       </c>
       <c r="I108" s="19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J108" s="3" t="s">
         <v>50</v>
@@ -10669,7 +10667,7 @@
         <v>20</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D109" s="19" t="s">
         <v>17</v>
@@ -10687,7 +10685,7 @@
         <v>96</v>
       </c>
       <c r="I109" s="19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J109" s="3" t="s">
         <v>50</v>
@@ -10767,7 +10765,7 @@
         <v>20</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D110" s="19" t="s">
         <v>17</v>
@@ -10785,7 +10783,7 @@
         <v>96</v>
       </c>
       <c r="I110" s="19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J110" s="3" t="s">
         <v>50</v>
@@ -10865,7 +10863,7 @@
         <v>20</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D111" s="19" t="s">
         <v>17</v>
@@ -10883,7 +10881,7 @@
         <v>96</v>
       </c>
       <c r="I111" s="19" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J111" s="3" t="s">
         <v>50</v>
@@ -10963,7 +10961,7 @@
         <v>20</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D112" s="8" t="s">
         <v>30</v>
@@ -10981,7 +10979,7 @@
         <v>96</v>
       </c>
       <c r="I112" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J112" s="3" t="s">
         <v>50</v>
@@ -11057,7 +11055,7 @@
         <v>20</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D113" s="8" t="s">
         <v>30</v>
@@ -11075,7 +11073,7 @@
         <v>96</v>
       </c>
       <c r="I113" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J113" s="3" t="s">
         <v>50</v>
@@ -11151,10 +11149,10 @@
         <v>20</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D114" s="19" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E114" s="19" t="s">
         <v>73</v>
@@ -11169,7 +11167,7 @@
         <v>96</v>
       </c>
       <c r="I114" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J114" s="3" t="s">
         <v>50</v>
@@ -11249,10 +11247,10 @@
         <v>20</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D115" s="19" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E115" s="19" t="s">
         <v>73</v>
@@ -11267,7 +11265,7 @@
         <v>96</v>
       </c>
       <c r="I115" s="19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J115" s="3" t="s">
         <v>50</v>
@@ -11347,10 +11345,10 @@
         <v>20</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D116" s="19" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E116" s="19" t="s">
         <v>73</v>
@@ -11365,7 +11363,7 @@
         <v>96</v>
       </c>
       <c r="I116" s="19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J116" s="3" t="s">
         <v>50</v>
@@ -11445,10 +11443,10 @@
         <v>20</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D117" s="19" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E117" s="19" t="s">
         <v>73</v>
@@ -11463,7 +11461,7 @@
         <v>96</v>
       </c>
       <c r="I117" s="19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J117" s="3" t="s">
         <v>50</v>
@@ -11543,10 +11541,10 @@
         <v>20</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D118" s="19" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E118" s="19" t="s">
         <v>73</v>
@@ -11561,7 +11559,7 @@
         <v>96</v>
       </c>
       <c r="I118" s="19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J118" s="3" t="s">
         <v>50</v>
@@ -11641,10 +11639,10 @@
         <v>20</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D119" s="19" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E119" s="19" t="s">
         <v>73</v>
@@ -11659,7 +11657,7 @@
         <v>96</v>
       </c>
       <c r="I119" s="19" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J119" s="3" t="s">
         <v>50</v>
@@ -11739,7 +11737,7 @@
         <v>20</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D120" s="3" t="s">
         <v>51</v>
@@ -11755,7 +11753,7 @@
       </c>
       <c r="H120" s="3"/>
       <c r="I120" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J120" s="3" t="s">
         <v>50</v>
@@ -11835,7 +11833,7 @@
         <v>20</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D121" s="3" t="s">
         <v>51</v>
@@ -11851,7 +11849,7 @@
       </c>
       <c r="H121" s="3"/>
       <c r="I121" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J121" s="3" t="s">
         <v>50</v>
@@ -11931,7 +11929,7 @@
         <v>20</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D122" s="3" t="s">
         <v>51</v>
@@ -11947,7 +11945,7 @@
       </c>
       <c r="H122" s="3"/>
       <c r="I122" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J122" s="3" t="s">
         <v>50</v>
@@ -12027,7 +12025,7 @@
         <v>20</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D123" s="3" t="s">
         <v>51</v>
@@ -12043,7 +12041,7 @@
       </c>
       <c r="H123" s="3"/>
       <c r="I123" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J123" s="3" t="s">
         <v>50</v>
@@ -12123,7 +12121,7 @@
         <v>20</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D124" s="3" t="s">
         <v>51</v>
@@ -12139,7 +12137,7 @@
       </c>
       <c r="H124" s="3"/>
       <c r="I124" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J124" s="3" t="s">
         <v>50</v>
@@ -12219,7 +12217,7 @@
         <v>20</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>51</v>
@@ -12235,7 +12233,7 @@
       </c>
       <c r="H125" s="3"/>
       <c r="I125" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J125" s="3" t="s">
         <v>50</v>
@@ -12312,10 +12310,10 @@
         <v>21</v>
       </c>
       <c r="B126" s="19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D126" s="19" t="s">
         <v>113</v>
@@ -12333,7 +12331,7 @@
         <v>96</v>
       </c>
       <c r="I126" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J126" s="19" t="s">
         <v>50</v>
@@ -12410,10 +12408,10 @@
         <v>21</v>
       </c>
       <c r="B127" s="19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D127" s="19" t="s">
         <v>113</v>
@@ -12431,7 +12429,7 @@
         <v>96</v>
       </c>
       <c r="I127" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J127" s="19" t="s">
         <v>50</v>
@@ -12508,10 +12506,10 @@
         <v>21</v>
       </c>
       <c r="B128" s="19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D128" s="19" t="s">
         <v>113</v>
@@ -12529,7 +12527,7 @@
         <v>96</v>
       </c>
       <c r="I128" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J128" s="19" t="s">
         <v>50</v>
@@ -12606,10 +12604,10 @@
         <v>21</v>
       </c>
       <c r="B129" s="19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D129" s="19" t="s">
         <v>113</v>
@@ -12627,7 +12625,7 @@
         <v>96</v>
       </c>
       <c r="I129" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J129" s="19" t="s">
         <v>50</v>
@@ -12704,10 +12702,10 @@
         <v>21</v>
       </c>
       <c r="B130" s="19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D130" s="19" t="s">
         <v>113</v>
@@ -12725,7 +12723,7 @@
         <v>96</v>
       </c>
       <c r="I130" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J130" s="19" t="s">
         <v>50</v>
@@ -12802,10 +12800,10 @@
         <v>21</v>
       </c>
       <c r="B131" s="19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D131" s="19" t="s">
         <v>113</v>
@@ -12823,7 +12821,7 @@
         <v>96</v>
       </c>
       <c r="I131" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J131" s="19" t="s">
         <v>50</v>
@@ -12903,7 +12901,7 @@
         <v>20</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D132" s="19" t="s">
         <v>114</v>
@@ -12921,7 +12919,7 @@
         <v>96</v>
       </c>
       <c r="I132" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J132" s="19" t="s">
         <v>50</v>
@@ -13001,7 +12999,7 @@
         <v>20</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D133" s="19" t="s">
         <v>114</v>
@@ -13019,7 +13017,7 @@
         <v>96</v>
       </c>
       <c r="I133" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J133" s="19" t="s">
         <v>50</v>
@@ -13099,7 +13097,7 @@
         <v>20</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D134" s="19" t="s">
         <v>114</v>
@@ -13117,7 +13115,7 @@
         <v>96</v>
       </c>
       <c r="I134" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J134" s="19" t="s">
         <v>50</v>
@@ -13197,7 +13195,7 @@
         <v>20</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D135" s="19" t="s">
         <v>114</v>
@@ -13215,7 +13213,7 @@
         <v>96</v>
       </c>
       <c r="I135" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J135" s="19" t="s">
         <v>50</v>
@@ -13295,7 +13293,7 @@
         <v>20</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D136" s="19" t="s">
         <v>114</v>
@@ -13313,7 +13311,7 @@
         <v>96</v>
       </c>
       <c r="I136" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J136" s="19" t="s">
         <v>50</v>
@@ -13393,7 +13391,7 @@
         <v>20</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D137" s="19" t="s">
         <v>114</v>
@@ -13411,7 +13409,7 @@
         <v>96</v>
       </c>
       <c r="I137" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J137" s="19" t="s">
         <v>50</v>
@@ -13491,7 +13489,7 @@
         <v>20</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D138" s="19" t="s">
         <v>111</v>
@@ -13509,7 +13507,7 @@
         <v>96</v>
       </c>
       <c r="I138" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J138" s="19" t="s">
         <v>50</v>
@@ -13589,7 +13587,7 @@
         <v>20</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D139" s="19" t="s">
         <v>111</v>
@@ -13607,7 +13605,7 @@
         <v>96</v>
       </c>
       <c r="I139" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J139" s="19" t="s">
         <v>50</v>
@@ -13687,7 +13685,7 @@
         <v>20</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D140" s="19" t="s">
         <v>111</v>
@@ -13705,7 +13703,7 @@
         <v>96</v>
       </c>
       <c r="I140" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J140" s="19" t="s">
         <v>50</v>
@@ -13785,7 +13783,7 @@
         <v>20</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D141" s="19" t="s">
         <v>111</v>
@@ -13803,7 +13801,7 @@
         <v>96</v>
       </c>
       <c r="I141" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J141" s="19" t="s">
         <v>50</v>
@@ -13883,7 +13881,7 @@
         <v>20</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D142" s="19" t="s">
         <v>111</v>
@@ -13901,7 +13899,7 @@
         <v>96</v>
       </c>
       <c r="I142" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J142" s="19" t="s">
         <v>50</v>
@@ -13981,7 +13979,7 @@
         <v>20</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D143" s="19" t="s">
         <v>111</v>
@@ -13999,7 +13997,7 @@
         <v>96</v>
       </c>
       <c r="I143" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J143" s="19" t="s">
         <v>50</v>
@@ -14079,10 +14077,10 @@
         <v>20</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D144" s="19" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E144" s="19" t="s">
         <v>77</v>
@@ -14173,10 +14171,10 @@
         <v>20</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D145" s="19" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E145" s="19" t="s">
         <v>77</v>
@@ -14267,10 +14265,10 @@
         <v>20</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D146" s="19" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E146" s="19" t="s">
         <v>77</v>
@@ -14361,10 +14359,10 @@
         <v>20</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D147" s="19" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E147" s="19" t="s">
         <v>77</v>
@@ -14455,10 +14453,10 @@
         <v>20</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D148" s="19" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E148" s="19" t="s">
         <v>77</v>
@@ -14549,10 +14547,10 @@
         <v>20</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D149" s="19" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E149" s="19" t="s">
         <v>77</v>
@@ -14643,7 +14641,7 @@
         <v>20</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D150" s="19" t="s">
         <v>3</v>
@@ -14737,7 +14735,7 @@
         <v>20</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D151" s="19" t="s">
         <v>3</v>
@@ -14831,7 +14829,7 @@
         <v>20</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D152" s="19" t="s">
         <v>3</v>
@@ -14925,7 +14923,7 @@
         <v>20</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D153" s="19" t="s">
         <v>3</v>
@@ -15019,7 +15017,7 @@
         <v>20</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D154" s="19" t="s">
         <v>3</v>
@@ -15113,7 +15111,7 @@
         <v>20</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D155" s="19" t="s">
         <v>3</v>
@@ -15222,7 +15220,7 @@
         <v>57</v>
       </c>
       <c r="H156" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I156" s="3"/>
       <c r="J156" s="3" t="s">
@@ -15294,7 +15292,7 @@
         <v>20</v>
       </c>
       <c r="D157" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E157" s="8" t="s">
         <v>73</v>
@@ -15306,7 +15304,7 @@
         <v>57</v>
       </c>
       <c r="H157" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I157" s="3"/>
       <c r="J157" s="3" t="s">
@@ -15402,10 +15400,10 @@
         <v>59</v>
       </c>
       <c r="H158" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I158" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J158" s="3" t="s">
         <v>50</v>
@@ -15666,7 +15664,7 @@
         <v>22</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C161" s="3" t="s">
         <v>20</v>
@@ -15748,7 +15746,7 @@
         <v>22</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C162" s="3" t="s">
         <v>20</v>
@@ -15840,7 +15838,7 @@
         <v>22</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C163" s="3" t="s">
         <v>20</v>
@@ -16443,7 +16441,7 @@
         <v>22</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C170" s="3" t="s">
         <v>20</v>
@@ -16645,7 +16643,7 @@
         <v>22</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C172" s="3" t="s">
         <v>20</v>
@@ -16775,7 +16773,7 @@
         <v>20</v>
       </c>
       <c r="D174" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E174" s="8" t="s">
         <v>74</v>
@@ -16790,7 +16788,7 @@
         <v>117</v>
       </c>
       <c r="I174" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J174" s="3" t="s">
         <v>50</v>
@@ -16855,13 +16853,13 @@
         <v>22</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C175" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D175" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E175" s="8" t="s">
         <v>74</v>
@@ -16873,7 +16871,7 @@
         <v>58</v>
       </c>
       <c r="H175" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I175" s="3"/>
       <c r="J175" s="3" t="s">
@@ -16939,7 +16937,7 @@
         <v>22</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C176" s="3" t="s">
         <v>20</v>
@@ -17025,7 +17023,7 @@
         <v>22</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C177" s="3" t="s">
         <v>20</v>
@@ -17087,13 +17085,13 @@
         <v>22</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C178" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D178" s="8" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E178" s="8" t="s">
         <v>74</v>
@@ -17106,7 +17104,7 @@
       </c>
       <c r="H178" s="7"/>
       <c r="I178" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="J178" s="3" t="s">
         <v>88</v>
@@ -17147,13 +17145,13 @@
         <v>22</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C179" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D179" s="8" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E179" s="8" t="s">
         <v>74</v>
@@ -17165,10 +17163,10 @@
         <v>59</v>
       </c>
       <c r="H179" s="7" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="I179" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J179" s="3" t="s">
         <v>50</v>
@@ -17245,7 +17243,7 @@
         <v>22</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C180" s="3" t="s">
         <v>20</v>
@@ -17337,7 +17335,7 @@
         <v>22</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C181" s="3" t="s">
         <v>20</v>
@@ -17481,7 +17479,7 @@
         <v>22</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C183" s="3" t="s">
         <v>20</v>
@@ -17576,19 +17574,19 @@
     </row>
     <row r="184" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A184" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B184" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D184" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="E184" s="23" t="s">
         <v>191</v>
-      </c>
-      <c r="B184" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C184" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D184" s="23" t="s">
-        <v>192</v>
-      </c>
-      <c r="E184" s="23" t="s">
-        <v>193</v>
       </c>
       <c r="F184" s="3" t="s">
         <v>63</v>
@@ -17597,10 +17595,10 @@
         <v>59</v>
       </c>
       <c r="H184" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I184" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J184" s="3" t="s">
         <v>50</v>
@@ -17674,7 +17672,7 @@
     </row>
     <row r="185" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A185" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B185" s="23" t="s">
         <v>20</v>
@@ -17683,7 +17681,7 @@
         <v>20</v>
       </c>
       <c r="D185" s="23" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E185" s="23" t="s">
         <v>74</v>
@@ -17753,19 +17751,19 @@
     </row>
     <row r="186" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A186" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D186" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="E186" s="23" t="s">
         <v>191</v>
-      </c>
-      <c r="B186" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="C186" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D186" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="E186" s="23" t="s">
-        <v>193</v>
       </c>
       <c r="F186" s="3" t="s">
         <v>63</v>
@@ -17774,10 +17772,10 @@
         <v>59</v>
       </c>
       <c r="H186" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I186" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J186" s="3" t="s">
         <v>50</v>
@@ -17858,7 +17856,7 @@
     </row>
     <row r="187" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A187" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B187" s="23" t="s">
         <v>35</v>
@@ -17867,10 +17865,10 @@
         <v>20</v>
       </c>
       <c r="D187" s="23" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E187" s="23" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F187" s="3" t="s">
         <v>63</v>
@@ -17879,10 +17877,10 @@
         <v>59</v>
       </c>
       <c r="H187" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="I187" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="I187" s="3" t="s">
-        <v>200</v>
       </c>
       <c r="J187" s="3" t="s">
         <v>50</v>
@@ -17963,19 +17961,19 @@
     </row>
     <row r="188" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A188" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B188" s="23" t="s">
+        <v>261</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D188" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="E188" s="23" t="s">
         <v>191</v>
-      </c>
-      <c r="B188" s="23" t="s">
-        <v>263</v>
-      </c>
-      <c r="C188" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D188" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="E188" s="23" t="s">
-        <v>193</v>
       </c>
       <c r="F188" s="3" t="s">
         <v>63</v>
@@ -17984,10 +17982,10 @@
         <v>59</v>
       </c>
       <c r="H188" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I188" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J188" s="3" t="s">
         <v>50</v>
@@ -18050,7 +18048,7 @@
     </row>
     <row r="189" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A189" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B189" s="23" t="s">
         <v>20</v>
@@ -18059,7 +18057,7 @@
         <v>20</v>
       </c>
       <c r="D189" s="23" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E189" s="23" t="s">
         <v>74</v>
@@ -18129,7 +18127,7 @@
     </row>
     <row r="190" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A190" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B190" s="23" t="s">
         <v>20</v>
@@ -18138,10 +18136,10 @@
         <v>20</v>
       </c>
       <c r="D190" s="23" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E190" s="23" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F190" s="3" t="s">
         <v>63</v>
@@ -18150,10 +18148,10 @@
         <v>59</v>
       </c>
       <c r="H190" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I190" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J190" s="3" t="s">
         <v>50</v>
@@ -18216,19 +18214,19 @@
     </row>
     <row r="191" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A191" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C191" s="23" t="s">
         <v>20</v>
       </c>
       <c r="D191" s="23" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E191" s="23" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F191" s="3"/>
       <c r="G191" s="3"/>
@@ -18295,7 +18293,7 @@
     </row>
     <row r="192" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A192" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B192" s="23" t="s">
         <v>20</v>
@@ -18304,10 +18302,10 @@
         <v>20</v>
       </c>
       <c r="D192" s="23" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E192" s="23" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F192" s="3"/>
       <c r="G192" s="3"/>
@@ -18374,7 +18372,7 @@
     </row>
     <row r="193" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A193" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B193" s="23" t="s">
         <v>35</v>
@@ -18383,10 +18381,10 @@
         <v>20</v>
       </c>
       <c r="D193" s="23" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E193" s="23" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F193" s="3" t="s">
         <v>60</v>
@@ -18395,7 +18393,7 @@
         <v>58</v>
       </c>
       <c r="H193" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I193" s="3"/>
       <c r="J193" s="3" t="s">
@@ -18459,19 +18457,19 @@
     </row>
     <row r="194" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A194" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B194" s="23" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C194" s="23" t="s">
         <v>20</v>
       </c>
       <c r="D194" s="23" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E194" s="23" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F194" s="3"/>
       <c r="G194" s="3"/>
@@ -18538,7 +18536,7 @@
     </row>
     <row r="195" spans="1:30" s="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A195" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B195" s="23" t="s">
         <v>28</v>
@@ -18547,10 +18545,10 @@
         <v>20</v>
       </c>
       <c r="D195" s="23" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E195" s="23" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F195" s="3" t="s">
         <v>60</v>
@@ -18559,10 +18557,10 @@
         <v>58</v>
       </c>
       <c r="H195" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I195" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J195" s="3" t="s">
         <v>50</v>
@@ -18643,19 +18641,19 @@
     </row>
     <row r="196" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A196" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C196" s="23" t="s">
         <v>20</v>
       </c>
       <c r="D196" s="23" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E196" s="23" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F196" s="3"/>
       <c r="G196" s="3"/>
@@ -18722,7 +18720,7 @@
     </row>
     <row r="197" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A197" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B197" s="23" t="s">
         <v>35</v>
@@ -18731,10 +18729,10 @@
         <v>20</v>
       </c>
       <c r="D197" s="23" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E197" s="23" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F197" s="3"/>
       <c r="G197" s="3"/>
@@ -18801,19 +18799,19 @@
     </row>
     <row r="198" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A198" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B198" s="23" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C198" s="23" t="s">
         <v>20</v>
       </c>
       <c r="D198" s="23" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E198" s="23" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F198" s="3"/>
       <c r="G198" s="3"/>
@@ -18880,7 +18878,7 @@
     </row>
     <row r="199" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A199" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B199" s="23" t="s">
         <v>28</v>
@@ -18889,10 +18887,10 @@
         <v>20</v>
       </c>
       <c r="D199" s="23" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E199" s="23" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F199" s="3"/>
       <c r="G199" s="3"/>
@@ -18959,19 +18957,19 @@
     </row>
     <row r="200" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A200" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C200" s="23" t="s">
         <v>20</v>
       </c>
       <c r="D200" s="23" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E200" s="23" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F200" s="3"/>
       <c r="G200" s="3"/>
@@ -19038,19 +19036,19 @@
     </row>
     <row r="201" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A201" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C201" s="23" t="s">
         <v>20</v>
       </c>
       <c r="D201" s="23" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E201" s="23" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F201" s="3"/>
       <c r="G201" s="3"/>
@@ -19117,19 +19115,19 @@
     </row>
     <row r="202" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A202" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B202" s="23" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C202" s="23" t="s">
         <v>20</v>
       </c>
       <c r="D202" s="23" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E202" s="23" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F202" s="3"/>
       <c r="G202" s="3"/>
@@ -19196,7 +19194,7 @@
     </row>
     <row r="203" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A203" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B203" s="23" t="s">
         <v>105</v>
@@ -19205,10 +19203,10 @@
         <v>20</v>
       </c>
       <c r="D203" s="23" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E203" s="23" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F203" s="3"/>
       <c r="G203" s="3"/>
@@ -19251,19 +19249,19 @@
     </row>
     <row r="204" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A204" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B204" s="23" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C204" s="23" t="s">
         <v>20</v>
       </c>
       <c r="D204" s="23" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E204" s="23" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F204" s="3"/>
       <c r="G204" s="3"/>
@@ -19330,7 +19328,7 @@
     </row>
     <row r="205" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A205" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B205" s="23" t="s">
         <v>28</v>
@@ -19339,10 +19337,10 @@
         <v>20</v>
       </c>
       <c r="D205" s="23" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E205" s="23" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F205" s="3"/>
       <c r="G205" s="3"/>
@@ -19409,7 +19407,7 @@
     </row>
     <row r="206" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A206" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B206" s="23" t="s">
         <v>27</v>
@@ -19418,10 +19416,10 @@
         <v>20</v>
       </c>
       <c r="D206" s="23" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E206" s="23" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F206" s="3"/>
       <c r="G206" s="3"/>
@@ -19488,19 +19486,19 @@
     </row>
     <row r="207" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A207" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B207" s="23" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C207" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D207" s="23" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E207" s="23" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F207" s="3"/>
       <c r="G207" s="3"/>
@@ -19567,19 +19565,19 @@
     </row>
     <row r="208" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A208" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C208" s="23" t="s">
         <v>20</v>
       </c>
       <c r="D208" s="23" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E208" s="23" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F208" s="3"/>
       <c r="G208" s="3"/>
@@ -19646,19 +19644,19 @@
     </row>
     <row r="209" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A209" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B209" s="23" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C209" s="23" t="s">
         <v>20</v>
       </c>
       <c r="D209" s="23" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E209" s="23" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F209" s="3" t="s">
         <v>62</v>
@@ -19668,7 +19666,7 @@
       </c>
       <c r="H209" s="3"/>
       <c r="I209" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J209" s="3" t="s">
         <v>50</v>
@@ -19734,71 +19732,70 @@
   <hyperlinks>
     <hyperlink ref="H158" r:id="rId1"/>
     <hyperlink ref="H89" r:id="rId2"/>
-    <hyperlink ref="H42" r:id="rId3"/>
-    <hyperlink ref="H180" r:id="rId4"/>
-    <hyperlink ref="H177" r:id="rId5"/>
-    <hyperlink ref="H176" r:id="rId6"/>
-    <hyperlink ref="H170" r:id="rId7"/>
-    <hyperlink ref="H171" r:id="rId8"/>
-    <hyperlink ref="H172" r:id="rId9"/>
-    <hyperlink ref="H173" r:id="rId10"/>
-    <hyperlink ref="H161" r:id="rId11"/>
-    <hyperlink ref="H112" r:id="rId12"/>
-    <hyperlink ref="H113" r:id="rId13"/>
-    <hyperlink ref="H159" r:id="rId14"/>
-    <hyperlink ref="H160" r:id="rId15"/>
-    <hyperlink ref="H45" r:id="rId16"/>
-    <hyperlink ref="H182" r:id="rId17"/>
-    <hyperlink ref="H4" r:id="rId18"/>
-    <hyperlink ref="H5" r:id="rId19"/>
-    <hyperlink ref="H6" r:id="rId20"/>
-    <hyperlink ref="H77" r:id="rId21"/>
-    <hyperlink ref="H78" r:id="rId22"/>
-    <hyperlink ref="H80" r:id="rId23"/>
-    <hyperlink ref="H82" r:id="rId24"/>
-    <hyperlink ref="H79" r:id="rId25"/>
-    <hyperlink ref="H81" r:id="rId26"/>
-    <hyperlink ref="H83" r:id="rId27"/>
-    <hyperlink ref="H84" r:id="rId28"/>
-    <hyperlink ref="H85" r:id="rId29"/>
-    <hyperlink ref="H86" r:id="rId30"/>
-    <hyperlink ref="H87" r:id="rId31"/>
-    <hyperlink ref="H88" r:id="rId32"/>
-    <hyperlink ref="H106:H111" r:id="rId33" display="https://ec.europa.eu/clima/sites/clima/files/transport/vehicles/heavy/docs/hdv_lightweighting_en.pdf"/>
-    <hyperlink ref="H126" r:id="rId34"/>
-    <hyperlink ref="H127" r:id="rId35"/>
-    <hyperlink ref="H128" r:id="rId36"/>
-    <hyperlink ref="H129" r:id="rId37"/>
-    <hyperlink ref="H130" r:id="rId38"/>
-    <hyperlink ref="H131" r:id="rId39"/>
-    <hyperlink ref="H132" r:id="rId40"/>
-    <hyperlink ref="H133" r:id="rId41"/>
-    <hyperlink ref="H134" r:id="rId42"/>
-    <hyperlink ref="H135" r:id="rId43"/>
-    <hyperlink ref="H136" r:id="rId44"/>
-    <hyperlink ref="H137" r:id="rId45"/>
-    <hyperlink ref="H138" r:id="rId46"/>
-    <hyperlink ref="H139" r:id="rId47"/>
-    <hyperlink ref="H140" r:id="rId48"/>
-    <hyperlink ref="H141" r:id="rId49"/>
-    <hyperlink ref="H142" r:id="rId50"/>
-    <hyperlink ref="H143" r:id="rId51"/>
-    <hyperlink ref="H156" r:id="rId52"/>
-    <hyperlink ref="H157" r:id="rId53"/>
-    <hyperlink ref="H18" r:id="rId54" location="bib41"/>
-    <hyperlink ref="H8" r:id="rId55"/>
-    <hyperlink ref="H7" r:id="rId56"/>
-    <hyperlink ref="H19" r:id="rId57" location="bib41"/>
-    <hyperlink ref="H20" r:id="rId58" location="bib41"/>
-    <hyperlink ref="H195" r:id="rId59"/>
-    <hyperlink ref="H114:H119" r:id="rId60" display="https://ec.europa.eu/clima/sites/clima/files/transport/vehicles/heavy/docs/hdv_lightweighting_en.pdf"/>
-    <hyperlink ref="H72" r:id="rId61"/>
-    <hyperlink ref="H15" r:id="rId62"/>
-    <hyperlink ref="H175" r:id="rId63"/>
-    <hyperlink ref="H57" r:id="rId64"/>
-    <hyperlink ref="H68:H70" r:id="rId65" display="https://pubs.acs.org/doi/pdf/10.1021/acsenergylett.7b00432"/>
+    <hyperlink ref="H180" r:id="rId3"/>
+    <hyperlink ref="H177" r:id="rId4"/>
+    <hyperlink ref="H176" r:id="rId5"/>
+    <hyperlink ref="H170" r:id="rId6"/>
+    <hyperlink ref="H171" r:id="rId7"/>
+    <hyperlink ref="H172" r:id="rId8"/>
+    <hyperlink ref="H173" r:id="rId9"/>
+    <hyperlink ref="H161" r:id="rId10"/>
+    <hyperlink ref="H112" r:id="rId11"/>
+    <hyperlink ref="H113" r:id="rId12"/>
+    <hyperlink ref="H159" r:id="rId13"/>
+    <hyperlink ref="H160" r:id="rId14"/>
+    <hyperlink ref="H45" r:id="rId15"/>
+    <hyperlink ref="H182" r:id="rId16"/>
+    <hyperlink ref="H4" r:id="rId17"/>
+    <hyperlink ref="H5" r:id="rId18"/>
+    <hyperlink ref="H6" r:id="rId19"/>
+    <hyperlink ref="H77" r:id="rId20"/>
+    <hyperlink ref="H78" r:id="rId21"/>
+    <hyperlink ref="H80" r:id="rId22"/>
+    <hyperlink ref="H82" r:id="rId23"/>
+    <hyperlink ref="H79" r:id="rId24"/>
+    <hyperlink ref="H81" r:id="rId25"/>
+    <hyperlink ref="H83" r:id="rId26"/>
+    <hyperlink ref="H84" r:id="rId27"/>
+    <hyperlink ref="H85" r:id="rId28"/>
+    <hyperlink ref="H86" r:id="rId29"/>
+    <hyperlink ref="H87" r:id="rId30"/>
+    <hyperlink ref="H88" r:id="rId31"/>
+    <hyperlink ref="H106:H111" r:id="rId32" display="https://ec.europa.eu/clima/sites/clima/files/transport/vehicles/heavy/docs/hdv_lightweighting_en.pdf"/>
+    <hyperlink ref="H126" r:id="rId33"/>
+    <hyperlink ref="H127" r:id="rId34"/>
+    <hyperlink ref="H128" r:id="rId35"/>
+    <hyperlink ref="H129" r:id="rId36"/>
+    <hyperlink ref="H130" r:id="rId37"/>
+    <hyperlink ref="H131" r:id="rId38"/>
+    <hyperlink ref="H132" r:id="rId39"/>
+    <hyperlink ref="H133" r:id="rId40"/>
+    <hyperlink ref="H134" r:id="rId41"/>
+    <hyperlink ref="H135" r:id="rId42"/>
+    <hyperlink ref="H136" r:id="rId43"/>
+    <hyperlink ref="H137" r:id="rId44"/>
+    <hyperlink ref="H138" r:id="rId45"/>
+    <hyperlink ref="H139" r:id="rId46"/>
+    <hyperlink ref="H140" r:id="rId47"/>
+    <hyperlink ref="H141" r:id="rId48"/>
+    <hyperlink ref="H142" r:id="rId49"/>
+    <hyperlink ref="H143" r:id="rId50"/>
+    <hyperlink ref="H156" r:id="rId51"/>
+    <hyperlink ref="H157" r:id="rId52"/>
+    <hyperlink ref="H18" r:id="rId53" location="bib41"/>
+    <hyperlink ref="H8" r:id="rId54"/>
+    <hyperlink ref="H7" r:id="rId55"/>
+    <hyperlink ref="H19" r:id="rId56" location="bib41"/>
+    <hyperlink ref="H20" r:id="rId57" location="bib41"/>
+    <hyperlink ref="H195" r:id="rId58"/>
+    <hyperlink ref="H114:H119" r:id="rId59" display="https://ec.europa.eu/clima/sites/clima/files/transport/vehicles/heavy/docs/hdv_lightweighting_en.pdf"/>
+    <hyperlink ref="H72" r:id="rId60"/>
+    <hyperlink ref="H15" r:id="rId61"/>
+    <hyperlink ref="H175" r:id="rId62"/>
+    <hyperlink ref="H57" r:id="rId63"/>
+    <hyperlink ref="H68:H70" r:id="rId64" display="https://pubs.acs.org/doi/pdf/10.1021/acsenergylett.7b00432"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId66"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId65"/>
 </worksheet>
 </file>
</xml_diff>